<commit_message>
Rearranged Mexico from Central to North America
</commit_message>
<xml_diff>
--- a/us_born_outside_us_links_w_state_compare.xlsx
+++ b/us_born_outside_us_links_w_state_compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\Dropbox\General Folder\Python\Git_projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1DB17B-029D-40EF-B63C-A5E4C701EE4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93FC79C-82B3-4F12-B4CD-6F717175DA67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3480" yWindow="15630" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NYTimes_2019_revenue_data_links" sheetId="1" r:id="rId1"/>
@@ -755,12 +755,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1124,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1892,7 @@
       <c r="B45">
         <v>32</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="5">
         <v>2383676</v>
       </c>
       <c r="D45" t="s">
@@ -1905,13 +1907,13 @@
         <v>37</v>
       </c>
       <c r="B46">
-        <v>36</v>
-      </c>
-      <c r="C46" s="1">
+        <v>44</v>
+      </c>
+      <c r="C46" s="5">
         <v>11171893</v>
       </c>
       <c r="D46" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -1924,7 +1926,7 @@
       <c r="B47">
         <v>36</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="5">
         <v>1419330</v>
       </c>
       <c r="D47" t="s">
@@ -1941,7 +1943,7 @@
       <c r="B48">
         <v>36</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="5">
         <v>2162417</v>
       </c>
       <c r="D48" t="s">
@@ -1958,7 +1960,7 @@
       <c r="B49">
         <v>40</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="5">
         <v>472637</v>
       </c>
       <c r="D49" t="s">
@@ -1975,7 +1977,7 @@
       <c r="B50">
         <v>40</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="6">
         <v>789561</v>
       </c>
       <c r="D50" t="s">
@@ -1992,7 +1994,7 @@
       <c r="B51">
         <v>40</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="5">
         <v>2040884</v>
       </c>
       <c r="D51" t="s">
@@ -2009,7 +2011,7 @@
       <c r="B52">
         <v>31</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="5">
         <v>4461065</v>
       </c>
       <c r="D52" t="s">
@@ -2026,8 +2028,8 @@
       <c r="B53">
         <v>31</v>
       </c>
-      <c r="C53" s="1">
-        <v>14753640</v>
+      <c r="C53" s="5">
+        <v>3581747</v>
       </c>
       <c r="D53" t="s">
         <v>71</v>
@@ -2043,7 +2045,7 @@
       <c r="B54">
         <v>31</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="6">
         <v>3303082</v>
       </c>
       <c r="D54" t="s">
@@ -2060,7 +2062,7 @@
       <c r="B55">
         <v>44</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="6">
         <v>813664</v>
       </c>
       <c r="D55" t="s">
@@ -2077,7 +2079,7 @@
       <c r="B56">
         <v>44</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="6">
         <v>8805</v>
       </c>
       <c r="D56" t="s">
@@ -2094,8 +2096,8 @@
       <c r="B57">
         <v>30</v>
       </c>
-      <c r="C57" s="1">
-        <v>22517787</v>
+      <c r="C57" s="5">
+        <v>11345894</v>
       </c>
       <c r="D57" t="s">
         <v>71</v>
@@ -2111,8 +2113,8 @@
       <c r="B58">
         <v>30</v>
       </c>
-      <c r="C58" s="1">
-        <v>822469</v>
+      <c r="C58" s="5">
+        <v>11994362</v>
       </c>
       <c r="D58" t="s">
         <v>67</v>
@@ -2128,7 +2130,7 @@
       <c r="B59">
         <v>47</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="4">
         <v>23340256</v>
       </c>
       <c r="D59" s="4" t="s">

</xml_diff>